<commit_message>
update cost factor description
</commit_message>
<xml_diff>
--- a/cb_factors/cost_factors.xlsx
+++ b/cb_factors/cost_factors.xlsx
@@ -5,16 +5,30 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="20"/>
   </bookViews>
   <sheets>
-    <sheet name="crops_trns_tech_costs" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="crops_trns_non_tech_benefits" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="lvst_trns_tech_costs" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="crosscuting_trns_tech_costs" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="crosscuting_trns_non_tech_benef" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="lndu_trns_cb" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="ind_trns_tech_costs" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="crops_trns_tech_costs" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="crops_trns_non_tech_benefits" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="lvst_trns_tech_costs" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="crosscuting_trns_tech_costs" sheetId="4" state="visible" r:id="rId6"/>
+    <sheet name="crosscuting_trns_non_tech_benef" sheetId="5" state="visible" r:id="rId7"/>
+    <sheet name="lndu_trns_cb" sheetId="6" state="visible" r:id="rId8"/>
+    <sheet name="ind_trns_tech_costs" sheetId="7" state="visible" r:id="rId9"/>
+    <sheet name="ind_trns_non_tech_costs_benefit" sheetId="8" state="visible" r:id="rId10"/>
+    <sheet name="energy_prod_trns_tech_costs" sheetId="9" state="visible" r:id="rId11"/>
+    <sheet name="energy_prod_trns_non_tech_costs" sheetId="10" state="visible" r:id="rId12"/>
+    <sheet name="building_trns_tech_costs" sheetId="11" state="visible" r:id="rId13"/>
+    <sheet name="transport_trns_tech_costs" sheetId="12" state="visible" r:id="rId14"/>
+    <sheet name="transport_trns_non_tech_costs" sheetId="13" state="visible" r:id="rId15"/>
+    <sheet name="wali_industrial" sheetId="14" state="visible" r:id="rId16"/>
+    <sheet name="wali_domestic" sheetId="15" state="visible" r:id="rId17"/>
+    <sheet name="wali_trns_tech_costs" sheetId="16" state="visible" r:id="rId18"/>
+    <sheet name="wali_trns_non_tech_costs" sheetId="17" state="visible" r:id="rId19"/>
+    <sheet name="waso_management_systems" sheetId="18" state="visible" r:id="rId20"/>
+    <sheet name="waso_trns_tech_costs" sheetId="19" state="visible" r:id="rId21"/>
+    <sheet name="waso_management_tech_costs" sheetId="20" state="visible" r:id="rId22"/>
+    <sheet name="waso_trns_non_tech_costs" sheetId="21" state="visible" r:id="rId23"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -26,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="236">
   <si>
     <t xml:space="preserve">Transformation</t>
   </si>
@@ -149,7 +163,7 @@
     <t xml:space="preserve">Increasing crop or livestock productivity</t>
   </si>
   <si>
-    <t xml:space="preserve"> Varies by country</t>
+    <t xml:space="preserve">- Varies by country</t>
   </si>
   <si>
     <t xml:space="preserve">This is deeply uncertain. As an initial estimate, we use the average annual investment in agriculture and livestock research and development (R&amp;D) in OECD countries, as a fraction of GDP (roughly 0.02%). We use that fraction for OECD countries in LAC; for others, we increase that fraction by 20% to account for less-developed economies.</t>
@@ -158,7 +172,7 @@
     <t xml:space="preserve">Change in sector value add</t>
   </si>
   <si>
-    <t xml:space="preserve">Price per ton varies by type of product</t>
+    <t xml:space="preserve">- Price per ton varies by type of product</t>
   </si>
   <si>
     <t xml:space="preserve">- Food waste occurs across food types, and without specific information on the types of food that are wasted and the recovery potential in the supply chain, we use the average cost of food across all product types. We reduce this value given that the food that is recovered from waste may be of lower value than food that is not wasted.</t>
@@ -167,7 +181,7 @@
     <t xml:space="preserve">Household grocery costs from improved diets</t>
   </si>
   <si>
-    <t xml:space="preserve">$385 per person per year transitioned to a better diet</t>
+    <t xml:space="preserve">- $385 per person per year transitioned to a better diet</t>
   </si>
   <si>
     <t xml:space="preserve">The annual cost of food in the improved diet described by Springmann et al., (2016) is less than the existing average diet, with food prices in LAC based on Springmann et al. (2017) and adjusted to 2019 dollars.</t>
@@ -176,7 +190,7 @@
     <t xml:space="preserve">Health benefits of better diets</t>
   </si>
   <si>
-    <t xml:space="preserve">$1,750/per person per year transitioned to a better diet
+    <t xml:space="preserve">- $1,750/per person per year transitioned to a better diet
 </t>
   </si>
   <si>
@@ -223,28 +237,9 @@
         <sz val="9"/>
         <rFont val="Arial"/>
         <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">Technical costs</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="9"/>
-        <rFont val="Arial"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">(LAC average in 2019 USD)
-</t>
+      <t xml:space="preserve">Technical costs (LAC average in 2019 USD) </t>
     </r>
     <r>
       <rPr>
@@ -337,6 +332,683 @@
     <t xml:space="preserve">The IEA (2020b) estimates that CCS globally adds $30-50/ton cement, $50/ton of steel, and $100/ton of chemicals.
 </t>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Value
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(LAC average in 2019 USD)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(Positive values indicate benefits and savings)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Avoided health effects from local air pollution from concrete production, excluding industrial energy pollution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- $45/ton cement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Miller et al., (2020, Figure 2) estimate cement externalities of $80-90/ton in Latin America in 2015 dollars, of which at least 75% stem from local air pollution’s health effects. Of this, at least 70% is from process-based (i.e., non-energy) emissions.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avoided health impacts from local air pollution from industrial on-site energy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- $2.47/GJ coal
+- $0.12/GJ natural gas 
+- $2.47/GJ coke (a coal-based fuel) 
+- $0.31/l diesel      
+- $0.039/l gasoline      
+- $3.05/GJ biomass
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We use IMF’s fossil-fuel subsidies database (2021) to calculate the avoided air pollution costs of industrial fuel consumption. This database provides costs specific to industry’s use of coal and natural gas. We use average values across LAC. We use coal costs for coke, and use costs shown in transport for diesel and gasoline. For biomass, we use average pollution costs across other fuel types.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transition to a renewable grid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Capex, non-fuel opex, and fuels are calculated endogenously
+- $2.70/MWh of new transmission
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NemoMod calculates the least-cost pathway to a renewable grid, including capital, operations and maintenance, and fuel costs.
+According to the National Renewable Energy Laboratory (Gorman et al., 2019), the levelized cost of new transmission in the US ranges from $1/MWh to $10/MWh. We use an average of $5/MWh and convert to LAC.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Produce green hydrogen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Endogenously calculated in NemoMod based on increased demand for renewable electricity to produce hydrogen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reduce transmission losses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Inter-American Development Bank (Brichettei et al., 2021) estimates the cost between 2020 and 2030 of upgrading each country’s grid to meet Sustainable Development Goals (SDGs) to 2030. We use a simple annual average as an approximation of the annual cost of upgrades in each country that would yield reductions in transmission losses.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minimize fugitive emissions leaks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- $20/tCO2e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Studies suggest that fugitive emissions could be abated for less than $14/tCO2e in the US oil and gas industry through various technologies (ICF International, 2014, Figures A-4 and A-5). We use a conservative estimate, given variations in discount rates, assumptions about methane prices, and so on.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flare fugitive emissions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- $2/tCO2e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We assume flaring will be one-tenth the cost of fixing leaks.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value
+(LAC average in 2019 USD)
+(Positive indicate benefits)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Health benefit of avoided air pollution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- $2.77/GJ coal
+- $0.99/GJ natural gas
+- $1.43/GJ oil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We use IMF’s fossil-fuel subsidies database (2021) to calculate the avoided air pollution costs of electricity generated by renewables versus coal, natural gas, and oil. (Costs are averaged across LAC, and the average cost of coal and natural gas is used for oil). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Improve building and appliance efficiency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- $0.02/kWh saved
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Perry et al. (2019, p. 17) estimate the costs in 2018 dollars of reducing building energy demands through a variety of energy-efficiency measures in the US (for purposes of comparing them to the costs of installing solar photovoltaic). We adjust the average cost effectiveness of $0.04/kWh saved for LAC.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transition heating to heat pumps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- $5/MWhth capital cost, reaching cost parity in 10 years
+- $0.90/MWhth non-fuel operations and maintenance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We use the same cost data as for low-temperature heat pumps used in industrial energy. Rissman (2022) estimates that heat pumps have a levelized capital cost of $8/MW of thermal heat demand compared to other technologies, but that this cost premium is shrinking rapidly, with a $1.50 savings in non-fuel opex in the US in 2022 dollars. (No discount rate is documented in this report, and we use levelized costs as presented).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Technical costs
+(LAC average in 2019)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electrify LDVs</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">- $0.039/vehicle-kilometer (vkm) in capital cost, declining over time
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">- $0.012/vkm in maintenance cost (i.e., savings)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">These costs reflect the marginal capital and maintenance costs of EVs versus internal combustion engine (ICE) LDVs per km. In the US, light-duty EVs are estimated to have $12,000 of higher up-front cost (Baik et al., 2019) than traditional LDVs and have $949/year lower maintenance costs (AAA, 2019) than their ICE counterparts. We approximate that charging infrastructure may involve an additional $1,000 in capital costs per EV, consistent with data from the US on the costs (Purnazeri, 2022) and deployment of charging stations (Evadoption, 2021). The per-km capital cost shown in the table assumes vehicles are driven 15,000 km/year (Ecola et al., 2008, Ecola et al, 2012, Ecola et al., 2014) and have a 12-year lifespan, consistent with data on vehicle lifetimes in the US (BTS, undated). Then costs are adjusted to 2019 costs for LAC.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fuel switch MDVs and HDVs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- $0.042/vkm + $0.011/kWh in capital cost, declining over time
+- $0.02/vkm in maintenance cost (i.e., savings)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Burke et al. (2022) provide marginal capital and maintenance costs of a variety of medium- and heavy-duty battery electric vehicles (BEVs) versus ICEs (Table 19a, p. 50), and the cost of charging infrastructure (p. 22). Using a stated 12-year lifetime, we calculate a simple average of these costs across all vehicle types. Then costs are adjusted to 2019 costs for LAC.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electrify rail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- $0.0013/metric ton per kilometer (mtkm) or pkm in capital cost
+- $0.0002/mtkm or pkm in maintenance cost (i.e., savings)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Popovich et al. (2021) estimate the capital and maintenance costs of electrifying freight rail. In absence of other information, we assume that electrifying passenger rail will have similar costs per person-km, with a lower mass of passengers compared to freight offset by climate control, lower density, and other variables.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fuel switch maritime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- $0.0005/mtkm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carlo et al. (2020) estimate that decarbonizing the maritime industry (using ammonia as the primary fuel) by 2050 will cost roughly $1 trillion, with 55% of that cost associated with ammonia production and storage and ship-related investments (Krantz et al, 2020). Here, 45% of the cost is associated with hydrogen production, which we account for in energy production. They also estimate a total demand of approximately 500,000-billion-tonnautical miles of demand. We use this data to approximate a cost of fuel switching per MTKM of total goods movement and apply this to LAC.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Increase energy efficiency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- $0.88M/PJ, equivalent to $0.002/vkm for ICE LDVs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The National Research Council (2015) estimates the technical cost and percent fuel economy improvements for LDVs from a wide range of vehicle technologies, including power train, accessories, and vehicle mass. We estimate the average cost per improvement across all technologies and calculate a per-km cost assuming a 12-year vehicle lifetime and 15,000 km/year use. Assuming a fuel economy of 12km/l, we calculate a cost per unit of energy saved and, in the absence of other data, apply this to other modes and fuel types.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Increase occupancy for private vehicles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There are no technical costs associated with increasing private vehicle occupancy; the savings (from avoided costs of transport by auto) are calculated in the system costs. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Mode shift freight 
+- Mode shift local and regional passenger travel
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The technical costs and savings of freight and passenger mode shifting are a combination of the following: the system cost for providing transport by different modes, the additional cost of expanding infrastructure associated with certain modes of the transport system (e.g., rail transport) to account for added demand; and the cost savings of avoided infrastructure expansion in modes with less demand (e.g., air transport). Quantifying these effects is deeply uncertain, highly localized, and beyond this study’s scope. We note, however, that mode shifts could result in a net cost savings, given that the shifts are generally from modes that are infrastructure inefficient (e.g., personal autos) to modes that are more infrastructure efficient (e.g., transit).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">System cost of passenger transport</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- $0.17/vkm for automobiles
+- $0.017/vkm for motorcycles
+- $5.20/vkm for bus
+- $14/vkm for passenger rail
+- $1067/vkm for aviation
+- (Transit cost is weighted assuming 75% bus, 25% rail)
+</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">The system cost of providing passenger transport will change as modes and demand change. We approximate this as the cost of vehicle ownership and operating costs. In the US, the capital and operating costs (excluding fuel) by mode are approximately: 
+$0.31/vkm for automobiles (US DOT National Transportation Statistics, undated, Table 3-17);
+$10/vkm on for buses (averaged across bus types) and $27/vkm (per passenger car) for passenger rail (averaged across rail types) (US FTA, 2021, Capital Expenses, Operating Expenses, and Metrics tables);
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">$2,000/vkm for aviation (calculated from US Department of Transportation </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">National Transportation Statistics</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">’ Tables 1-35, 1-40, and 3-20, assuming 10% of costs are for fuel); and 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">$0.031/vkm for powered bikes, which we assume are one-tenth the cost of automobiles. 
+Note that different modes may include infrastructure costs to different degrees – the cost of transport infrastructure is largely external to automobile owner/operating costs, whereas it is more likely to be internalized for air transport costs. We adapt these costs to Latin America. 
+</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">System cost of freight transport</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+- $0.41/mtkm for air
+- $0.053/mtkm for truck
+- $0.014/mtkm for rail
+- $0.01/mtkm for water
+</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">We estimate the impact of mode shifting freight based on costs associated with freight transport in the US ($0.86/mtkm by air; $0.11/mtkm by truck; 0.03/mtkm by rail, and $0.02/mtkm by water) and adjust to LAC (US Department of Transportation’s </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">National Transportation Statistics</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">, undated, Table 3-21). We exclude fuel costs, assuming they account for 10% of the reported revenue cost. Note that different modes may include infrastructure costs to different degrees – the cost of transport infrastructure is largely external to automobile owner/operating costs, whereas it is more likely to be internalized for air transport costs.
+</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">- $0.039/l gasoline and biofuels     
+- $0.31/l diesel
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We use IMF’s fossil fuel subsidies database (2021) to estimate the avoided air pollution costs of fossil fuels used for road transport, averaged across LAC.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avoided external crashes and congestion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Crash costs 
+- $0.33/l gasoline and biofuels   
+- $0.17/l diesel
+- $0.008/kwh electricity       
+- Congestion costs
+- $0.19/l gasoline and biofuels      
+- $0.17/l diesel
+- $0.005/kwh electricity
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We use IMF’s fossil-fuel subsidies database (2021) to estimate the avoided congestion and crash cost on roads. These costs are provided per liter of fuel and reflect external costs. We use average costs across LAC and calculate total crash costs assuming external crash costs are 75% of the total (Parry et al., 2014). We assume gasoline externalities apply to biofuels and we apply costs to EVs by calculating the cost per unit of energy, adjusting for approximately 4× higher energy efficiency of EVs. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Treatment system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No treatment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wastewater is not treated and is discharged into the environment.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Primary treatment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wastewater first is submitted to preliminary treatment to remove grit, rags, and large solids (e.g., wood or plastic) followed by primary treatment.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Secondary treatment
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wastewater is treated at a wastewater treatment plant and includes preliminary, primary, and secondary treatment.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tertiary treatment (aerobic)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wastewater is treated at an aerobic wastewater treatment plant and includes preliminary, primary, secondary, and tertiary treatment. Sludge is diverted further and managed as solid waste in the solid waste model.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tertiary treatment (anaerobic)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wastewater is treated at an anaerobic wastewater treatment plant and includes preliminary, primary, secondary, and tertiary treatment.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sanitation system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rural</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Urban</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unimproved sanitation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Open defecation (OD) or basic latrines without wastewater treatment, corresponding to the lowest two rungs of the Joint Monitoring Program (JMP) sanitation ladder (unimproved and limited sanitation). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Improved  sanitation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">On-site treatment in basic septic tanks or improved latrines, corresponding to the middle two rungs of the JMP sanitation ladder (improved and basic sanitation).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">On-site treatment in basic septic tanks or sewered collection without subsequent wastewater treatment, corresponding to the middle two rungs of the JMP sanitation ladder (improved and basic sanitation).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Safely managed sanitation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Septic tanks or improved latrines with fecal sludge management (FSM), consistent with the definition of “safely managed sanitation” used by the JMP.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sewered collection with subsequent centralized treatment at a wastewater treatment facility (see Table B.1), consistent with the definition of “safely managed sanitation” used by the JMP. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wastewater management system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Technical costs
+(LAC average in 2019 USD)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Domestic rural and urban sanitation :
+- Unimproved sanitation (rural)
+- Improved sanitation (rural)
+- Safely managed sanitation (rural)
+- Unimproved sanitation (urban)
+- Improved sanitation (urban)
+- Safely managed sanitation  (urban, sanitation only)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- $6.5/capita/year
+- $68.1/capita/year
+- $102.1/capita/year
+- $6.5/capita/year
+- $34.1/capita/year
+- $66.2/capita/year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Domestic sanitation and wastewater treatment costs are based on Tables D.1 and E.1 in Hutton &amp; Varughese (2016), Table A.4.1 in Brichetti et al. (2021), Table 1 in Dodane et al. (2012), and Daudey (2018). Average wastewater produced in LAC is based on Table 4 in Jones et al. (2021). We assume industrial wastewater treatment costs the same as domestic wastewater treatment per quantity of treated water. The full cost of safely managed sanitation in urban settings is the cost of the sanitation system (per capita) and the cost of treating the collected wastewater (per m3) using one of the wastewater treatment systems.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Industrial and domestic urban wastewater treatment:
+- No treatment
+- Primary
+- Secondary (aerobic)
+- Secondary (anaerobic)
+- Tertiary (aerobic)
+- Tertiary (anaerobic)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- $[0.02, 0.06, 0.30]/m3
+- $[0.24, 0.64, 3.10]/m3
+- $[0.40, 0.80, 3.27]/m3 
+- $[0.40, 0.80, 3.27]/m3 
+- $[0.80, 1.60, 6.54]/m3
+- $[0.80, 1.60, 6.54]/m3
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Domestic sanitation and wastewater treatment costs are based on Tables D.1 and E.1 in Hutton &amp; Varughese (2016), Table A.4.1 in Brichetti et al. (2021), Table 1 in Dodane et al. (2012), and Daudey (2018). Average wastewater produced in LAC is based on Table 4 in Jones et al. (2021). Here, the costs are given for each treatment option in isolation. So, wastewater that receives tertiary treatment will also receive primary and secondary treatment and incur those costs. 
+We assume industrial wastewater treatment costs the same as domestic wastewater treatment per quantity of treated water. The cost of no treatment is the cost of collecting industrial wastewater and dumping it untreated into waterways. We estimated it as one-tenth the cost of sewerage (i.e., safely managed urban sanitation) on a per cubic meter basis.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Biogas capture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$17/million British thermal units (MBtu) of biogas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IEA (2020f) provides a global average cost of biogas capture at wastewater treatment facilities of $10.30/MBTU in capex and $4.30/MBTU in opex, which we convert to 2019 dollars in LAC.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Benefit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data source</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Improvements in health and productivity from better household sanitation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- $200/year/person transitioned to safe sanitation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The per capita benefits were calculated by dividing the total annual benefit of transitioning from unimproved to improved sanitation in LAC (Table 9) by the total population receiving improved sanitation interventions in LAC (Table 1) in Hutton (2012), adjusted from 2010 to 2019 dollars. The sanitation ladder in Hutton (2012) calculates the benefits of moving from unimproved to improved sanitation, but where the latter term could be extended to include (i.e., safely managed) sanitation options of septic tanks and sewerage with wastewater treatment without affecting the value of benefits. We therefore assume that the benefits roughly apply to transitions from unimproved to safely managed sanitation and improved to safely managed sanitation.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Health, environment, and productivity benefits of improved water quality from more and better wastewater treatment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- $51/kg P
+- $20/kg N
+- $0.13/kg of chemical oxygen demand (COD)
+- $0.06/kg of biological oxygen demand (BOD)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Several studies (Hernández-Sancho et al. (2010, 2015) and Antalová and Haluš (2020) calculate the value of BOD, COD, N, and phosphorous (P) removed from wastewater effluent. We use average values and adjust to LAC in 2019.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value of CH4 captured and used for energy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Endogenously valued in the energy sector model</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solid waste management</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Open dump </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unmanaged</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unmanaged discharge of solid waste (e.g., into above-ground piles, holes in the ground, or dumping into natural features such as ravines)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Open burning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unmanaged combustion of waste (e.g., in open air or open dumps, where emissions are directly released into the air)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Landfilling, with methane capture and flaring or reuse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Managed landfill</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solid waste collected and deposited in managed sites. This category includes different levels of methane and capture and flaring or reuse, the latter of which is an input into the energy sector.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">composting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Managed biological treatment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diverting organic matter for biological treatment, where degradable organic carbon largely is converted to CO2. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anaerobic biogas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diverting organic matter to anaerobic biogas facilities, which expedites the natural decomposition of organic material without oxygen to generate CH4, which can be recovered for energy and is an input into the energy sector.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recycling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diversion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diverting paper, plastics, and other waste materials to reuse in industrial processes.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Waste reduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Annualized technical costs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data sources and notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Retail and consumer food Waste reduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$100/ton of food waste avoided</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Costs are based on the average per-ton costs of consumer-facing actions to reduce food waste in the US found in the appendix of ReFED (2016), adjusted to LAC.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Waste management</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Technical costs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Collection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- $86/ton of waste</t>
+  </si>
+  <si>
+    <t xml:space="preserve">World Bank (2012) provides costs for collecting and managing waste for countries of different income groups. We use a LAC average to average costs between lower-middle and upper-middle income countries. We assume 70% of recycled and open dumped waste in LAC is collected, and 100% of waste in other management systems is collected. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Management</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- $10/ton—open dumping
+- $57/ton—managed landfill
+- $61/ton—composting
+- $86/ton—anaerobic biogas
+- $72/ton—recycling
+- $70/ton—incineration
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">World Bank (2012) provides costs for collecting and managing waste for countries of different income groups. We use a LAC average to average costs between lower-middle and upper-middle income countries. We assume 70% of recycled and open dumped waste in LAC is collected, and 100% of waste in other management systems is collected. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Energy recovery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- $170/ton waste feedstock (incineration)
+- $500/ton of gas recovered (landfills, anaerobic digesters)
+ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">For management without energy recovery, we use average costs across the lower-middle and upper-middle income tiers. The recycling cost includes the cost of separation and materials recovery. The processing and manufacturing costs are included in the value of recyclables (discussed in benefits) and estimated from the EPA’s documentation of paper recycling costs (EPA, 2019). 
+Cost for energy recovery is based on IEA estimates (2020f).
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Benefit category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Benefit value or valuation method</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value of waste avoided</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- $700/ton of food waste avoided
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Food waste occurs across food types, and without specific information on the types of food that are wasted and have recovery potential in the supply chain, we use the average price of food across all product types.
+ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reduced environmental and health impacts from open dumps to managed systems</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- $115/ton of unmanaged waste transitioned to managed pathways</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wilson et al. (2015) suggest a “conservative” cost of $20-50/capita/year from unmanaged waste and describe an average waste of 220 kg/capita/year among the poorest. We calculate costs assuming $20/capita and 0.22 ton/capita, adjusted from 2015 to 2019 dollars.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value of CH4 captured in landfills and used for energy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Endogenously assessed in the energy model</t>
+  </si>
 </sst>
 </file>
 
@@ -345,7 +1017,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -394,15 +1066,25 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <i val="true"/>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
       <sz val="9"/>
       <name val="Arial"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="9"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="1"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -413,7 +1095,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -456,6 +1138,20 @@
       <bottom style="thin"/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -482,7 +1178,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="42">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -543,36 +1239,112 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -585,6 +1357,112 @@
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
+</file>
+
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -653,6 +1531,771 @@
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="26.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="35.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="52.33"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="115.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>106</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="33.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="34.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="57.34"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="43.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="121.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="126.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>112</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="27.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="37.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="55.64"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="169.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="84.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="85.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="112.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="103.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="101.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="B7" s="28"/>
+      <c r="C7" s="17" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="123.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="B8" s="28"/>
+      <c r="C8" s="17" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="63" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="17"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="17"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="34.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="59.97"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>133</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="211.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="110.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="80.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="199.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>144</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="30.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="84.24"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="29" t="s">
+        <v>145</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="51.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="58.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="62.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="53.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="61.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>156</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="26.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="47.68"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>158</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="91.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="103.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="91.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>167</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="34.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="69.09"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="B1" s="32" t="s">
+        <v>169</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="180.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="33" t="s">
+        <v>170</v>
+      </c>
+      <c r="B2" s="33" t="s">
+        <v>171</v>
+      </c>
+      <c r="C2" s="34" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="148" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="33" t="s">
+        <v>173</v>
+      </c>
+      <c r="B3" s="35" t="s">
+        <v>174</v>
+      </c>
+      <c r="C3" s="36" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="53.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="37" t="s">
+        <v>176</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>177</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>178</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="23.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="29.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="75.35"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="19" t="s">
+        <v>179</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>180</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="116.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>183</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="138.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="17" t="s">
+        <v>185</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="81.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="22" t="s">
+        <v>188</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>189</v>
+      </c>
+      <c r="C4" s="22"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="24.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="79.22"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="29" t="s">
+        <v>190</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>191</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="49.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="17" t="s">
+        <v>192</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>193</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="65.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="17" t="s">
+        <v>195</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>193</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="55.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="17" t="s">
+        <v>197</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>198</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="59.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>201</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="58.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="17" t="s">
+        <v>203</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>201</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="55.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="17" t="s">
+        <v>205</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>206</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>207</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="25.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="35.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="54.1"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="29" t="s">
+        <v>208</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>209</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="114.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="38" t="s">
+        <v>211</v>
+      </c>
+      <c r="B2" s="38" t="s">
+        <v>212</v>
+      </c>
+      <c r="C2" s="39" t="s">
+        <v>213</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -722,6 +2365,158 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="26.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="36.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="69.02"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="24" t="s">
+        <v>214</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>215</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="64.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="40" t="s">
+        <v>216</v>
+      </c>
+      <c r="B2" s="40" t="s">
+        <v>217</v>
+      </c>
+      <c r="C2" s="40" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="126.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="84.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="17" t="s">
+        <v>222</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C5" s="41" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C6" s="41"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="23.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="32.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="69.32"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="24" t="s">
+        <v>226</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>227</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="79.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="17" t="s">
+        <v>228</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>229</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="87.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="17" t="s">
+        <v>231</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>232</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="80.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="22" t="s">
+        <v>234</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>235</v>
+      </c>
+      <c r="C4" s="22"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -803,7 +2598,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -813,7 +2608,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="65.88"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="43.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -876,7 +2671,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -943,11 +2738,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="36.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="34.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="34.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="31.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="36.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="34.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="34.77"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1017,115 +2812,115 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="Z1:AB9"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Z1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AA3" activeCellId="0" sqref="AA3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="51.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="67.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="71.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="51.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="67.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="71.57"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="33.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z1" s="19" t="s">
+    <row r="1" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="AA1" s="20" t="s">
+      <c r="B1" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="AB1" s="16" t="s">
+      <c r="C1" s="21" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="100.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="Z2" s="17" t="s">
+      <c r="A2" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="AA2" s="17" t="s">
+      <c r="B2" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="AB2" s="21" t="s">
+      <c r="C2" s="7" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="78" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="Z3" s="17" t="s">
+      <c r="A3" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="AA3" s="17" t="s">
+      <c r="B3" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="AB3" s="21" t="s">
+      <c r="C3" s="7" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="75.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="Z4" s="17" t="s">
+      <c r="A4" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="AA4" s="17" t="s">
+      <c r="B4" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="AB4" s="21" t="s">
+      <c r="C4" s="7" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="71.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="Z5" s="17" t="s">
+      <c r="A5" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="AA5" s="17" t="s">
+      <c r="B5" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="AB5" s="17" t="s">
+      <c r="C5" s="17" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="84.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="Z6" s="17" t="s">
+      <c r="A6" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="AA6" s="17" t="s">
+      <c r="B6" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="AB6" s="17" t="s">
+      <c r="C6" s="17" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="71.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="Z7" s="17" t="s">
+      <c r="A7" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="AA7" s="17" t="s">
+      <c r="B7" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="AB7" s="21" t="s">
+      <c r="C7" s="7" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="54.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="Z8" s="17" t="s">
+      <c r="A8" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="AA8" s="17" t="s">
+      <c r="B8" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="AB8" s="17" t="s">
+      <c r="C8" s="17" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="116" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="Z9" s="22" t="s">
+      <c r="A9" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="AA9" s="22" t="s">
+      <c r="B9" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="AB9" s="22" t="s">
+      <c r="C9" s="22" t="s">
         <v>82</v>
       </c>
     </row>
@@ -1138,4 +2933,159 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="32.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="35.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="47.75"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="133.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="137.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>89</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="38.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="52.7"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="43.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="75.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="51.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" s="26"/>
+    </row>
+    <row r="4" customFormat="false" ht="73.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="68.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="40.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>102</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>